<commit_message>
Update fin prot - Guillaume Gégo 8h36
</commit_message>
<xml_diff>
--- a/Excel/ADN.xlsx
+++ b/Excel/ADN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guill\VirtualBox VMs\SciViews Box 2020\shared\projects\TP-Bioch-BAB2-Q1\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33750DB-F718-498F-8CF1-8749638647D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5ED3AE-B056-43B1-A83B-849499EFA320}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{58E2A8D9-AE62-4847-B1C5-3548FF4B9A82}"/>
+    <workbookView xWindow="20505" yWindow="3435" windowWidth="18480" windowHeight="10545" xr2:uid="{58E2A8D9-AE62-4847-B1C5-3548FF4B9A82}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>

</xml_diff>